<commit_message>
update qa bugfix - IOBalance-Testing-v5 - 11/5/2017
</commit_message>
<xml_diff>
--- a/PLMVCSolution/PL.MVC.IOBalanceV2/Content/excel/templates/PurchaseOrderExcelTemplate.xlsx
+++ b/PLMVCSolution/PL.MVC.IOBalanceV2/Content/excel/templates/PurchaseOrderExcelTemplate.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lep.ridad\Documents\Visual Studio 2013\Projects\PLMVCSolution\PL.MVC.IOBalanceV2\Content\excel\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -15,8 +10,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,8 +36,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,7 +128,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,7 +163,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,21 +340,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -367,7 +362,7 @@
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>